<commit_message>
Update excel Method added in excel Helper
</commit_message>
<xml_diff>
--- a/POMfamework/src/main/java/com/POMfamework/helper/excelData/Data.xlsx
+++ b/POMfamework/src/main/java/com/POMfamework/helper/excelData/Data.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\POMFramework\POMfamework\src\main\java\com\POMfamework\helper\excelData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E9BDD4-A176-47B2-B2EA-D62D96A90D0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A340532E-B33C-4FCF-8817-638137CF5B07}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="3690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="TestResult" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>TestName</t>
   </si>
@@ -89,12 +84,19 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,21 +458,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1205B53-88F6-4B83-A466-F1D3E4B61B79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -498,7 +500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -512,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -526,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -547,19 +549,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E9747F-369D-4D44-BE0D-D2123403CAD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -567,19 +569,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>